<commit_message>
change template of NATALEE trial for an example
</commit_message>
<xml_diff>
--- a/datasets/Trial Data _ NATALEE.xlsx
+++ b/datasets/Trial Data _ NATALEE.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kailash/R/Breaking-ICE/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8159D16-0411-5F42-84D4-FA5C3C8DEA3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D12C046-DB12-A345-8B7C-C4B3B36BBBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
     <sheet name="Times" sheetId="2" r:id="rId2"/>
     <sheet name="EXP" sheetId="3" r:id="rId3"/>
     <sheet name="CON" sheetId="4" r:id="rId4"/>
+    <sheet name="weblink" sheetId="5" r:id="rId5"/>
+    <sheet name="sensitivity" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
   <si>
     <t>Use this file structure to load your own data into the Breaking ICE app and simulate different censoring types.</t>
   </si>
@@ -89,12 +91,30 @@
   <si>
     <t>CONy</t>
   </si>
+  <si>
+    <t>https://www.nejm.org/doi/full/10.1056/NEJMoa2305488</t>
+  </si>
+  <si>
+    <t>Experimental</t>
+  </si>
+  <si>
+    <t>type censoring (toxicity = T, disappointment = D)</t>
+  </si>
+  <si>
+    <t>percent censoring (between 0 and 100)</t>
+  </si>
+  <si>
+    <t>time frame max (from 0 to ?, in Months)</t>
+  </si>
+  <si>
+    <t>Control arm</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -128,6 +148,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -149,12 +177,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -7287,7 +7316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B1073"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:B419"/>
     </sheetView>
   </sheetViews>
@@ -13268,4 +13297,77 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C159BFD1-7E02-CC48-85B4-5AB8B8504F78}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D41B7AA-3818-684F-8570-E6541A00FE39}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
adding support for Sensitivity sheet in Trial data
</commit_message>
<xml_diff>
--- a/datasets/Trial Data _ NATALEE.xlsx
+++ b/datasets/Trial Data _ NATALEE.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kailash/R/Breaking-ICE/datasets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomann/projects/hug/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D12C046-DB12-A345-8B7C-C4B3B36BBBB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211D6871-9769-9345-96E0-B86B654B4E4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13140" yWindow="880" windowWidth="30240" windowHeight="17640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ReadMe" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="EXP" sheetId="3" r:id="rId3"/>
     <sheet name="CON" sheetId="4" r:id="rId4"/>
     <sheet name="weblink" sheetId="5" r:id="rId5"/>
-    <sheet name="sensitivity" sheetId="6" r:id="rId6"/>
+    <sheet name="Sensitivity" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>Use this file structure to load your own data into the Breaking ICE app and simulate different censoring types.</t>
   </si>
@@ -95,19 +95,34 @@
     <t>https://www.nejm.org/doi/full/10.1056/NEJMoa2305488</t>
   </si>
   <si>
-    <t>Experimental</t>
+    <t>Toxicity</t>
   </si>
   <si>
-    <t>type censoring (toxicity = T, disappointment = D)</t>
+    <t>Disappontment</t>
   </si>
   <si>
-    <t>percent censoring (between 0 and 100)</t>
+    <t>Parameter</t>
   </si>
   <si>
-    <t>time frame max (from 0 to ?, in Months)</t>
+    <t>Comment</t>
   </si>
   <si>
-    <t>Control arm</t>
+    <t>time_frame_max</t>
+  </si>
+  <si>
+    <t>from 0 to ?, in Months</t>
+  </si>
+  <si>
+    <t>modelling_type</t>
+  </si>
+  <si>
+    <t>percentage</t>
+  </si>
+  <si>
+    <t>type of censoring: Toxicity or Disappointment</t>
+  </si>
+  <si>
+    <t>percent censoring, between 0 and 100</t>
   </si>
 </sst>
 </file>
@@ -13319,53 +13334,84 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D41B7AA-3818-684F-8570-E6541A00FE39}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2">
+        <v>25</v>
+      </c>
+      <c r="D2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>23</v>
-      </c>
+        <v>28</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>30</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>